<commit_message>
excel sheet for data
</commit_message>
<xml_diff>
--- a/Labor2_Graphen_Ergebnisse.xlsx
+++ b/Labor2_Graphen_Ergebnisse.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippgehrig/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6F1F8494-915B-CB44-BC90-A5330028E3D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2D07A58-83FD-804D-83D4-8946D7E0F99B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="3000" windowWidth="28040" windowHeight="17440" activeTab="3" xr2:uid="{28BA3105-05C1-E144-B1EA-F4C034B57166}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="4" xr2:uid="{28BA3105-05C1-E144-B1EA-F4C034B57166}"/>
   </bookViews>
   <sheets>
     <sheet name="Versuch 1" sheetId="1" r:id="rId1"/>
     <sheet name="Versuch 2" sheetId="2" r:id="rId2"/>
     <sheet name="Versuch 3" sheetId="3" r:id="rId3"/>
     <sheet name="Versuch 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Versuch6" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>Vpp (gemessen)</t>
   </si>
@@ -96,14 +97,49 @@
   </si>
   <si>
     <t>3,9k</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>ua</t>
+  </si>
+  <si>
+    <t>Grenzfrequenz</t>
+  </si>
+  <si>
+    <t>ue</t>
+  </si>
+  <si>
+    <t>av</t>
+  </si>
+  <si>
+    <t>av expected</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -131,9 +167,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +598,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58024677-9551-B142-9C07-AC42D68163C5}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
@@ -822,4 +859,513 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05801C49-DAC1-204A-AC2E-FDA9E772F1BB}">
+  <dimension ref="A1:E33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C2">
+        <v>1.94</v>
+      </c>
+      <c r="D2">
+        <f>B2/C2</f>
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <f>($B$31/$B$32)*(1/(1+2*PI()*A2*$B$31*$B$33))</f>
+        <v>9.9375604660902521</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>20</v>
+      </c>
+      <c r="B3">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C3">
+        <v>1.94</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D26" si="0">B3/C3</f>
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E26" si="1">($B$31/$B$32)*(1/(1+2*PI()*A3*$B$31*$B$33))</f>
+        <v>9.8758958328160276</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C4">
+        <v>1.94</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="1"/>
+        <v>9.6954097204857863</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>100</v>
+      </c>
+      <c r="B5">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="C5">
+        <v>1.94</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="1"/>
+        <v>9.4088260255825098</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>200</v>
+      </c>
+      <c r="B6">
+        <v>19.3</v>
+      </c>
+      <c r="C6">
+        <v>1.94</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>9.9484536082474229</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="1"/>
+        <v>8.8836478829534027</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>500</v>
+      </c>
+      <c r="B7">
+        <v>18.7</v>
+      </c>
+      <c r="C7">
+        <v>1.94</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>9.6391752577319583</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="1"/>
+        <v>7.6094277638931178</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>16.8</v>
+      </c>
+      <c r="C8">
+        <v>1.94</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>8.6597938144329909</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="1"/>
+        <v>6.1413045490496243</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>2000</v>
+      </c>
+      <c r="B9">
+        <v>12.22</v>
+      </c>
+      <c r="C9">
+        <v>1.94</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>6.2989690721649492</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="1"/>
+        <v>4.4313727585582221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>5000</v>
+      </c>
+      <c r="B10">
+        <v>5.99</v>
+      </c>
+      <c r="C10">
+        <v>1.94</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>3.0876288659793816</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="1"/>
+        <v>2.4145300700522387</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>10000</v>
+      </c>
+      <c r="B11">
+        <v>3.14</v>
+      </c>
+      <c r="C11">
+        <v>1.94</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>1.6185567010309279</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="1"/>
+        <v>1.3730256169841295</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>20000</v>
+      </c>
+      <c r="B12">
+        <v>1.63</v>
+      </c>
+      <c r="C12">
+        <v>1.94</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>0.84020618556701032</v>
+      </c>
+      <c r="E12">
+        <f t="shared" si="1"/>
+        <v>0.73711682249161115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>50000</v>
+      </c>
+      <c r="B13">
+        <v>0.68</v>
+      </c>
+      <c r="C13">
+        <v>1.94</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>0.3505154639175258</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="1"/>
+        <v>0.30849033387726366</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>100000</v>
+      </c>
+      <c r="B14">
+        <v>0.34</v>
+      </c>
+      <c r="C14">
+        <v>1.94</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>0.1752577319587629</v>
+      </c>
+      <c r="E14">
+        <f t="shared" si="1"/>
+        <v>0.15666159634676979</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1200</v>
+      </c>
+      <c r="B17">
+        <v>15.7</v>
+      </c>
+      <c r="C17">
+        <v>1.94</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>8.0927835051546388</v>
+      </c>
+      <c r="E17">
+        <f t="shared" si="1"/>
+        <v>5.7013120143641141</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1300</v>
+      </c>
+      <c r="B18">
+        <v>15.2</v>
+      </c>
+      <c r="C18">
+        <v>1.94</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>7.8350515463917523</v>
+      </c>
+      <c r="E18">
+        <f t="shared" si="1"/>
+        <v>5.5041404926394382</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1400</v>
+      </c>
+      <c r="B19">
+        <v>14.6</v>
+      </c>
+      <c r="C19">
+        <v>1.94</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>7.5257731958762886</v>
+      </c>
+      <c r="E19">
+        <f t="shared" si="1"/>
+        <v>5.320150870547562</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1500</v>
+      </c>
+      <c r="B20">
+        <v>14.3</v>
+      </c>
+      <c r="C20">
+        <v>1.94</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>7.3711340206185572</v>
+      </c>
+      <c r="E20">
+        <f t="shared" si="1"/>
+        <v>5.1480639934192158</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="2">
+        <v>1591</v>
+      </c>
+      <c r="B21">
+        <v>13.9</v>
+      </c>
+      <c r="C21">
+        <v>1.94</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>7.1649484536082477</v>
+      </c>
+      <c r="E21">
+        <f t="shared" si="1"/>
+        <v>5.0008631930640499</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1700</v>
+      </c>
+      <c r="B22">
+        <v>13.4</v>
+      </c>
+      <c r="C22">
+        <v>1.94</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>6.9072164948453612</v>
+      </c>
+      <c r="E22">
+        <f t="shared" si="1"/>
+        <v>4.8352590909583135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1800</v>
+      </c>
+      <c r="B23">
+        <v>13</v>
+      </c>
+      <c r="C23">
+        <v>1.94</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>6.7010309278350517</v>
+      </c>
+      <c r="E23">
+        <f t="shared" si="1"/>
+        <v>4.6926912413826063</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1900</v>
+      </c>
+      <c r="B24">
+        <v>12.6</v>
+      </c>
+      <c r="C24">
+        <v>1.94</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>6.4948453608247423</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="1"/>
+        <v>4.5582898435439523</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>2000</v>
+      </c>
+      <c r="B25">
+        <v>12.22</v>
+      </c>
+      <c r="C25">
+        <v>1.94</v>
+      </c>
+      <c r="D25">
+        <f>B25/C26</f>
+        <v>6.2989690721649492</v>
+      </c>
+      <c r="E25">
+        <f t="shared" si="1"/>
+        <v>4.4313727585582221</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1600</v>
+      </c>
+      <c r="B26">
+        <v>13.9</v>
+      </c>
+      <c r="C26">
+        <v>1.94</v>
+      </c>
+      <c r="D26">
+        <f>B26/C26</f>
+        <v>7.1649484536082477</v>
+      </c>
+      <c r="E26">
+        <f t="shared" si="1"/>
+        <v>4.9867610242862295</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>15700</v>
+      </c>
+      <c r="D29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>25</v>
+      </c>
+      <c r="B31">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>26</v>
+      </c>
+      <c r="B32">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" t="s">
+        <v>27</v>
+      </c>
+      <c r="B33">
+        <v>1E-8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>